<commit_message>
Se realizan cambios y se agregan 3 casos de prueba como demo
</commit_message>
<xml_diff>
--- a/src/main/resources/fixtures/ReporteData.xlsx
+++ b/src/main/resources/fixtures/ReporteData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MI BANCO\new Android\mibanco-selenium\src\main\resources\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TSOFT ASIGNACIONES\PROYECTO XRAY\REPOSITORIO\tsoft-framework-web-23\src\main\resources\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0EAC5CD-D532-4FCA-B7C3-B9A45B8FD7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B7A6ED-4A98-4D03-BBE4-A0AEA1D3C30E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12495" yWindow="1125" windowWidth="15075" windowHeight="13665" xr2:uid="{072E0A59-470E-434C-8292-A5F603352FD5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{072E0A59-470E-434C-8292-A5F603352FD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Informe" sheetId="2" r:id="rId1"/>
@@ -87,13 +87,13 @@
     <t>Nombre de Aplicación o Módulo</t>
   </si>
   <si>
-    <t>Proyecto App Mobil Mi Banco</t>
-  </si>
-  <si>
-    <t>Mi Banco</t>
-  </si>
-  <si>
-    <t>Casos de pruebas del app movil mi banco</t>
+    <t>Proyecto TSOFT</t>
+  </si>
+  <si>
+    <t>TSOFT</t>
+  </si>
+  <si>
+    <t>Casos de pruebas para proyecto TSOFT</t>
   </si>
 </sst>
 </file>

</xml_diff>